<commit_message>
added ability for tkinter to open excel file
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -8,24 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\japes\Projects\scheduler.py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A67841F-C96C-4FD9-9598-37DB8021F1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0E1B16-C3A2-4D3A-A14E-1B2E40E08336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9150" yWindow="3045" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="employees" sheetId="1" r:id="rId1"/>
+    <sheet name="availability" sheetId="2" r:id="rId2"/>
+    <sheet name="positions" sheetId="3" r:id="rId3"/>
+    <sheet name="shifts" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>john</t>
   </si>
@@ -37,6 +51,12 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>luis</t>
+  </si>
+  <si>
+    <t>position</t>
   </si>
 </sst>
 </file>
@@ -354,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,7 +402,409 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09AD8062-FF99-47B5-95E9-C6D200DBFE0D}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>employees!A2</f>
+        <v>john</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>employees!A3</f>
+        <v>sharon</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>employees!A4</f>
+        <v>hannah</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>employees!A5</f>
+        <v>luis</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>employees!A6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>employees!A7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>employees!A8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>employees!A9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>employees!A10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>employees!A11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>employees!A12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>employees!A13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>employees!A14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>employees!A15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>employees!A16</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F074D5-1F69-402D-BB90-4B783E0B48BB}">
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>employees!A2</f>
+        <v>john</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>employees!A3</f>
+        <v>sharon</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>employees!A4</f>
+        <v>hannah</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>employees!A5</f>
+        <v>luis</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>employees!A6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>employees!A7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>employees!A8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>employees!A9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>employees!A10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>employees!A11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>employees!A12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>employees!A13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>employees!A14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>employees!A15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f>employees!A16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>employees!A17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f>employees!A18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f>employees!A19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f>employees!A20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>employees!A21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f>employees!A22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f>employees!A23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f>employees!A24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f>employees!A25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f>employees!A26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f>employees!A27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f>employees!A28</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f>employees!A29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>employees!A30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>employees!A31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f>employees!A32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f>employees!A33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f>employees!A34</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f>employees!A35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>employees!A36</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f>employees!A37</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>employees!A38</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f>employees!A39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f>employees!A40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f>employees!A41</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f>employees!A42</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f>employees!A43</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BEA11B5-9ADA-4CA4-8ACC-0EBF1688D1EA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
gave up on tkinter for now.
</commit_message>
<xml_diff>
--- a/employees.xlsx
+++ b/employees.xlsx
@@ -1,43 +1,88 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27716"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\japes\Projects\scheduler.py\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3E0FB1-AA07-4A3B-9324-224CAF29F1DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>luis</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>sharon</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>crew</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>hannah</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>hourly</t>
+  </si>
+  <si>
+    <t>salaried</t>
+  </si>
+  <si>
+    <t>josh</t>
+  </si>
+  <si>
+    <t>logan</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,94 +90,26 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,59 +397,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>luis</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>john</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>sharon</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>sharon1</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>sharon11</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>